<commit_message>
Added part number in the annexure file and show annexure in the invoice page
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/partner_inventory_invoice_annexure-v1.xlsx
+++ b/application/controllers/excel-templates/partner_inventory_invoice_annexure-v1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ANNEXURE</t>
   </si>
@@ -61,10 +61,16 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Part Number</t>
+  </si>
+  <si>
     <t>{booking:incoming_invoice_id}</t>
   </si>
   <si>
     <t>{booking:qty}</t>
+  </si>
+  <si>
+    <t>{booking:part_number}</t>
   </si>
 </sst>
 </file>
@@ -228,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -298,15 +304,6 @@
     <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -314,10 +311,7 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -524,30 +518,32 @@
       <c r="D16" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
+      <c r="E16" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="31" t="s">
+      <c r="B17" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="33"/>
+      <c r="D17" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -1530,11 +1526,13 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B12:G13"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Change Invoice generation process for returned Defective inventory #CRM-1010
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/partner_inventory_invoice_annexure-v1.xlsx
+++ b/application/controllers/excel-templates/partner_inventory_invoice_annexure-v1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ANNEXURE</t>
   </si>
@@ -58,19 +58,31 @@
     <t>Reference Invoice</t>
   </si>
   <si>
+    <t>Booking ID</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>Part Number</t>
+    <t>Rate</t>
   </si>
   <si>
     <t>{booking:incoming_invoice_id}</t>
   </si>
   <si>
+    <t>{booking:booking_id}</t>
+  </si>
+  <si>
+    <t>{booking:part_number}</t>
+  </si>
+  <si>
     <t>{booking:qty}</t>
   </si>
   <si>
-    <t>{booking:part_number}</t>
+    <t>{booking:rate}</t>
   </si>
 </sst>
 </file>
@@ -132,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border/>
     <border>
       <left style="thin">
@@ -210,6 +222,11 @@
       <top/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -234,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -242,7 +259,7 @@
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -301,25 +318,28 @@
     <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="13" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -346,9 +366,9 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="2.14"/>
     <col customWidth="1" min="2" max="2" width="14.14"/>
-    <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="6" width="18.57"/>
-    <col customWidth="1" min="7" max="7" width="14.14"/>
+    <col customWidth="1" min="3" max="4" width="16.0"/>
+    <col customWidth="1" min="5" max="7" width="18.57"/>
+    <col customWidth="1" min="8" max="8" width="14.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -359,6 +379,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -369,7 +390,8 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -378,7 +400,8 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="6"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -387,9 +410,10 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="6"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
@@ -399,10 +423,11 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
@@ -412,10 +437,11 @@
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
@@ -425,10 +451,11 @@
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -436,8 +463,9 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="6"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -445,8 +473,9 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
@@ -456,10 +485,11 @@
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15"/>
+      <c r="G10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
@@ -468,11 +498,12 @@
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="16"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
@@ -483,12 +514,13 @@
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="22"/>
-      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
@@ -498,52 +530,65 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="29" t="s">
+      <c r="B17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="12"/>
+      <c r="D17" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
       <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -1527,12 +1572,12 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B12:G13"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B12:H13"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>